<commit_message>
Updated Distrito Federal for Ciudad de México
</commit_message>
<xml_diff>
--- a/Mexican States.xlsx
+++ b/Mexican States.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielsalazar/repos/mexico-states/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C6A4A2D-C676-CC47-8C40-5F4A61AC4DD2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795C15CD-1E60-AD46-8F1D-AC7F949C41D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{ABE574D8-805A-8740-B9E6-EC2CB6D9D395}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="17040" xr2:uid="{ABE574D8-805A-8740-B9E6-EC2CB6D9D395}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Aguascalientes</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Zacatecas</t>
+  </si>
+  <si>
+    <t>Ciudad de México</t>
   </si>
 </sst>
 </file>
@@ -179,9 +182,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -219,7 +222,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -325,7 +328,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -467,7 +470,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A7A284C-E48F-F04B-AC54-A29922B65FDD}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A31"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,126 +518,131 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>